<commit_message>
Added metadata into database pipeline
</commit_message>
<xml_diff>
--- a/data/manual_changes/manual_awards.xlsx
+++ b/data/manual_changes/manual_awards.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="174">
   <si>
     <t>show</t>
   </si>
@@ -132,7 +132,7 @@
     <t>Rhapsody Of Sadness</t>
   </si>
   <si>
-    <t>Joezuz</t>
+    <t>ZOZAZZ</t>
   </si>
   <si>
     <t>Don't you know</t>
@@ -210,7 +210,7 @@
     <t>Love or Die</t>
   </si>
   <si>
-    <t>Jia</t>
+    <t>ZiA</t>
   </si>
   <si>
     <t>Tired of falling in love</t>
@@ -507,6 +507,18 @@
     <t>Tiger (New Flavour)</t>
   </si>
   <si>
+    <t>G-DRAGON &amp; V.A.</t>
+  </si>
+  <si>
+    <t>GOOD DAY 2025</t>
+  </si>
+  <si>
+    <t>KUN8</t>
+  </si>
+  <si>
+    <t>Wild Heart</t>
+  </si>
+  <si>
     <t>Hwang Karam</t>
   </si>
   <si>
@@ -516,7 +528,13 @@
     <t>JAECHAN</t>
   </si>
   <si>
-    <t>n.SSign</t>
+    <t>n.Ssign</t>
+  </si>
+  <si>
+    <t>G-Dragon</t>
+  </si>
+  <si>
+    <t>LUN8</t>
   </si>
 </sst>
 </file>
@@ -553,7 +571,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="15">
     <border/>
     <border>
       <left style="thin">
@@ -751,53 +769,11 @@
         <color rgb="FF284E3F"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF284E3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -852,6 +828,9 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -900,31 +879,19 @@
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1018,7 +985,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G26" displayName="Table2" name="Table2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G29" displayName="Table2" name="Table2" id="2">
   <tableColumns count="7">
     <tableColumn name="show" id="1"/>
     <tableColumn name="date" id="2"/>
@@ -1033,7 +1000,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G26" displayName="Table3" name="Table3" id="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G29" displayName="Table3" name="Table3" id="3">
   <tableColumns count="7">
     <tableColumn name="show" id="1"/>
     <tableColumn name="date" id="2"/>
@@ -2205,25 +2172,25 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="15">
         <v>45732.0</v>
       </c>
-      <c r="C42" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="D42" s="7" t="s">
+      <c r="C42" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="D42" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F42" s="17">
         <v>3186.0</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="G42" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2320,22 +2287,22 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="19">
+      <c r="B47" s="20">
         <v>44939.0</v>
       </c>
-      <c r="C47" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D47" s="21" t="s">
+      <c r="C47" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D47" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="E47" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F47" s="21">
+      <c r="F47" s="22">
         <v>6534.0</v>
       </c>
       <c r="G47" s="13" t="s">
@@ -2366,22 +2333,22 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="19">
+      <c r="B49" s="20">
         <v>44953.0</v>
       </c>
-      <c r="C49" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D49" s="21" t="s">
+      <c r="C49" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D49" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="21" t="s">
+      <c r="E49" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F49" s="21">
+      <c r="F49" s="22">
         <v>6831.0</v>
       </c>
       <c r="G49" s="13" t="s">
@@ -2412,22 +2379,22 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="18" t="s">
+      <c r="A51" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="19">
+      <c r="B51" s="20">
         <v>44967.0</v>
       </c>
-      <c r="C51" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D51" s="21" t="s">
+      <c r="C51" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D51" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E51" s="21" t="s">
+      <c r="E51" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F51" s="21">
+      <c r="F51" s="22">
         <v>7643.0</v>
       </c>
       <c r="G51" s="13" t="s">
@@ -2458,22 +2425,22 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B53" s="19">
+      <c r="B53" s="20">
         <v>44981.0</v>
       </c>
-      <c r="C53" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D53" s="21" t="s">
+      <c r="C53" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D53" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E53" s="21" t="s">
+      <c r="E53" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F53" s="21">
+      <c r="F53" s="22">
         <v>5682.0</v>
       </c>
       <c r="G53" s="13" t="s">
@@ -2504,22 +2471,22 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="18" t="s">
+      <c r="A55" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B55" s="19">
+      <c r="B55" s="20">
         <v>44995.0</v>
       </c>
-      <c r="C55" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D55" s="21" t="s">
+      <c r="C55" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D55" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E55" s="21" t="s">
+      <c r="E55" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F55" s="21">
+      <c r="F55" s="22">
         <v>4050.0</v>
       </c>
       <c r="G55" s="13" t="s">
@@ -2550,22 +2517,22 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="18" t="s">
+      <c r="A57" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B57" s="19">
+      <c r="B57" s="20">
         <v>45009.0</v>
       </c>
-      <c r="C57" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D57" s="21" t="s">
+      <c r="C57" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D57" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E57" s="21" t="s">
+      <c r="E57" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F57" s="21">
+      <c r="F57" s="22">
         <v>4492.0</v>
       </c>
       <c r="G57" s="13" t="s">
@@ -2596,22 +2563,22 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="18" t="s">
+      <c r="A59" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B59" s="19">
+      <c r="B59" s="20">
         <v>45023.0</v>
       </c>
-      <c r="C59" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D59" s="21" t="s">
+      <c r="C59" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D59" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E59" s="21" t="s">
+      <c r="E59" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F59" s="21">
+      <c r="F59" s="22">
         <v>6370.0</v>
       </c>
       <c r="G59" s="13" t="s">
@@ -2642,22 +2609,22 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="18" t="s">
+      <c r="A61" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B61" s="19">
+      <c r="B61" s="20">
         <v>45037.0</v>
       </c>
-      <c r="C61" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D61" s="21" t="s">
+      <c r="C61" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D61" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E61" s="21" t="s">
+      <c r="E61" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F61" s="21">
+      <c r="F61" s="22">
         <v>5410.0</v>
       </c>
       <c r="G61" s="13" t="s">
@@ -2688,22 +2655,22 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="18" t="s">
+      <c r="A63" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="19">
+      <c r="B63" s="20">
         <v>45051.0</v>
       </c>
-      <c r="C63" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D63" s="21" t="s">
+      <c r="C63" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D63" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E63" s="21" t="s">
+      <c r="E63" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F63" s="21">
+      <c r="F63" s="22">
         <v>5768.0</v>
       </c>
       <c r="G63" s="13" t="s">
@@ -2734,22 +2701,22 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B65" s="19">
+      <c r="B65" s="20">
         <v>45268.0</v>
       </c>
-      <c r="C65" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D65" s="21" t="s">
+      <c r="C65" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D65" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="E65" s="21" t="s">
+      <c r="E65" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F65" s="21">
+      <c r="F65" s="22">
         <v>2289.0</v>
       </c>
       <c r="G65" s="13" t="s">
@@ -2780,22 +2747,22 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="18" t="s">
+      <c r="A67" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="19">
+      <c r="B67" s="20">
         <v>44965.0</v>
       </c>
-      <c r="C67" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D67" s="21" t="s">
+      <c r="C67" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D67" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E67" s="21" t="s">
+      <c r="E67" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F67" s="21">
+      <c r="F67" s="22">
         <v>4359.0</v>
       </c>
       <c r="G67" s="13" t="s">
@@ -2826,22 +2793,22 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="18" t="s">
+      <c r="A69" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B69" s="19">
+      <c r="B69" s="20">
         <v>44972.0</v>
       </c>
-      <c r="C69" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D69" s="21" t="s">
+      <c r="C69" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D69" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E69" s="21" t="s">
+      <c r="E69" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F69" s="21">
+      <c r="F69" s="22">
         <v>3800.0</v>
       </c>
       <c r="G69" s="13" t="s">
@@ -2872,22 +2839,22 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="18" t="s">
+      <c r="A71" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B71" s="19">
+      <c r="B71" s="20">
         <v>44979.0</v>
       </c>
-      <c r="C71" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D71" s="21" t="s">
+      <c r="C71" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D71" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E71" s="21" t="s">
+      <c r="E71" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F71" s="21">
+      <c r="F71" s="22">
         <v>5997.0</v>
       </c>
       <c r="G71" s="13" t="s">
@@ -2918,22 +2885,22 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="18" t="s">
+      <c r="A73" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B73" s="19">
+      <c r="B73" s="20">
         <v>44986.0</v>
       </c>
-      <c r="C73" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D73" s="21" t="s">
+      <c r="C73" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D73" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E73" s="21" t="s">
+      <c r="E73" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F73" s="21">
+      <c r="F73" s="22">
         <v>4128.0</v>
       </c>
       <c r="G73" s="13" t="s">
@@ -2964,22 +2931,22 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="18" t="s">
+      <c r="A75" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B75" s="19">
+      <c r="B75" s="20">
         <v>44993.0</v>
       </c>
-      <c r="C75" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D75" s="21" t="s">
+      <c r="C75" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D75" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="E75" s="21" t="s">
+      <c r="E75" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="F75" s="21">
+      <c r="F75" s="22">
         <v>4255.0</v>
       </c>
       <c r="G75" s="13" t="s">
@@ -3010,22 +2977,22 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="18" t="s">
+      <c r="A77" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B77" s="19">
+      <c r="B77" s="20">
         <v>45007.0</v>
       </c>
-      <c r="C77" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D77" s="21" t="s">
+      <c r="C77" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D77" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="E77" s="21" t="s">
+      <c r="E77" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="F77" s="21">
+      <c r="F77" s="22">
         <v>3500.0</v>
       </c>
       <c r="G77" s="13" t="s">
@@ -3056,22 +3023,22 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="18" t="s">
+      <c r="A79" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B79" s="19">
+      <c r="B79" s="20">
         <v>45014.0</v>
       </c>
-      <c r="C79" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D79" s="21" t="s">
+      <c r="C79" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D79" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="E79" s="21" t="s">
+      <c r="E79" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F79" s="21">
+      <c r="F79" s="22">
         <v>7386.0</v>
       </c>
       <c r="G79" s="13" t="s">
@@ -3102,22 +3069,22 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="18" t="s">
+      <c r="A81" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B81" s="19">
+      <c r="B81" s="20">
         <v>45021.0</v>
       </c>
-      <c r="C81" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D81" s="21" t="s">
+      <c r="C81" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D81" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="E81" s="21" t="s">
+      <c r="E81" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F81" s="21">
+      <c r="F81" s="22">
         <v>5159.0</v>
       </c>
       <c r="G81" s="13" t="s">
@@ -3148,22 +3115,22 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="18" t="s">
+      <c r="A83" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B83" s="19">
+      <c r="B83" s="20">
         <v>45028.0</v>
       </c>
-      <c r="C83" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D83" s="21" t="s">
+      <c r="C83" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D83" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="E83" s="21" t="s">
+      <c r="E83" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F83" s="21">
+      <c r="F83" s="22">
         <v>3878.0</v>
       </c>
       <c r="G83" s="13" t="s">
@@ -3194,22 +3161,22 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="18" t="s">
+      <c r="A85" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B85" s="19">
+      <c r="B85" s="20">
         <v>45035.0</v>
       </c>
-      <c r="C85" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D85" s="21" t="s">
+      <c r="C85" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D85" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="E85" s="21" t="s">
+      <c r="E85" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="F85" s="21">
+      <c r="F85" s="22">
         <v>4684.0</v>
       </c>
       <c r="G85" s="13" t="s">
@@ -3240,22 +3207,22 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="18" t="s">
+      <c r="A87" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B87" s="19">
+      <c r="B87" s="20">
         <v>45042.0</v>
       </c>
-      <c r="C87" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D87" s="21" t="s">
+      <c r="C87" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D87" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E87" s="21" t="s">
+      <c r="E87" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F87" s="21">
+      <c r="F87" s="22">
         <v>4695.0</v>
       </c>
       <c r="G87" s="13" t="s">
@@ -3286,22 +3253,22 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="18" t="s">
+      <c r="A89" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B89" s="19">
+      <c r="B89" s="20">
         <v>45049.0</v>
       </c>
-      <c r="C89" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D89" s="21" t="s">
+      <c r="C89" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D89" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E89" s="21" t="s">
+      <c r="E89" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F89" s="21">
+      <c r="F89" s="22">
         <v>3742.0</v>
       </c>
       <c r="G89" s="13" t="s">
@@ -3332,22 +3299,22 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="18" t="s">
+      <c r="A91" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B91" s="19">
+      <c r="B91" s="20">
         <v>45056.0</v>
       </c>
-      <c r="C91" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D91" s="21" t="s">
+      <c r="C91" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D91" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E91" s="21" t="s">
+      <c r="E91" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F91" s="21">
+      <c r="F91" s="22">
         <v>3923.0</v>
       </c>
       <c r="G91" s="13" t="s">
@@ -3378,22 +3345,22 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="18" t="s">
+      <c r="A93" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B93" s="19">
+      <c r="B93" s="20">
         <v>45070.0</v>
       </c>
-      <c r="C93" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D93" s="21" t="s">
+      <c r="C93" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D93" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E93" s="21" t="s">
+      <c r="E93" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F93" s="21">
+      <c r="F93" s="22">
         <v>4726.0</v>
       </c>
       <c r="G93" s="13" t="s">
@@ -3424,13 +3391,13 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="18" t="s">
+      <c r="A95" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B95" s="19">
+      <c r="B95" s="20">
         <v>45105.0</v>
       </c>
-      <c r="C95" s="20">
+      <c r="C95" s="21">
         <v>2.0</v>
       </c>
       <c r="D95" s="12" t="s">
@@ -3470,22 +3437,22 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="18" t="s">
+      <c r="A97" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B97" s="19">
+      <c r="B97" s="20">
         <v>44933.0</v>
       </c>
-      <c r="C97" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D97" s="21" t="s">
+      <c r="C97" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D97" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="E97" s="21" t="s">
+      <c r="E97" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="F97" s="21">
+      <c r="F97" s="22">
         <v>5157.0</v>
       </c>
       <c r="G97" s="13" t="s">
@@ -3516,22 +3483,22 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="18" t="s">
+      <c r="A99" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B99" s="19">
+      <c r="B99" s="20">
         <v>44940.0</v>
       </c>
-      <c r="C99" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D99" s="21" t="s">
+      <c r="C99" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D99" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="E99" s="21" t="s">
+      <c r="E99" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="F99" s="21">
+      <c r="F99" s="22">
         <v>4706.0</v>
       </c>
       <c r="G99" s="13" t="s">
@@ -3562,22 +3529,22 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="18" t="s">
+      <c r="A101" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B101" s="19">
+      <c r="B101" s="20">
         <v>44954.0</v>
       </c>
-      <c r="C101" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D101" s="21" t="s">
+      <c r="C101" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D101" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E101" s="21" t="s">
+      <c r="E101" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F101" s="21">
+      <c r="F101" s="22">
         <v>5098.0</v>
       </c>
       <c r="G101" s="13" t="s">
@@ -3608,22 +3575,22 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="18" t="s">
+      <c r="A103" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B103" s="19">
+      <c r="B103" s="20">
         <v>44961.0</v>
       </c>
-      <c r="C103" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D103" s="21" t="s">
+      <c r="C103" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D103" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E103" s="21" t="s">
+      <c r="E103" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F103" s="21">
+      <c r="F103" s="22">
         <v>4816.0</v>
       </c>
       <c r="G103" s="13" t="s">
@@ -3654,22 +3621,22 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="18" t="s">
+      <c r="A105" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B105" s="19">
+      <c r="B105" s="20">
         <v>44968.0</v>
       </c>
-      <c r="C105" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D105" s="21" t="s">
+      <c r="C105" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D105" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E105" s="21" t="s">
+      <c r="E105" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F105" s="21">
+      <c r="F105" s="22">
         <v>5103.0</v>
       </c>
       <c r="G105" s="13" t="s">
@@ -3700,22 +3667,22 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="18" t="s">
+      <c r="A107" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B107" s="19">
+      <c r="B107" s="20">
         <v>44975.0</v>
       </c>
-      <c r="C107" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D107" s="21" t="s">
+      <c r="C107" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D107" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E107" s="21" t="s">
+      <c r="E107" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F107" s="21">
+      <c r="F107" s="22">
         <v>5785.0</v>
       </c>
       <c r="G107" s="13" t="s">
@@ -3746,22 +3713,22 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="18" t="s">
+      <c r="A109" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B109" s="19">
+      <c r="B109" s="20">
         <v>44982.0</v>
       </c>
-      <c r="C109" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D109" s="21" t="s">
+      <c r="C109" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D109" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E109" s="21" t="s">
+      <c r="E109" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F109" s="21">
+      <c r="F109" s="22">
         <v>5793.0</v>
       </c>
       <c r="G109" s="13" t="s">
@@ -3792,22 +3759,22 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="18" t="s">
+      <c r="A111" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B111" s="19">
+      <c r="B111" s="20">
         <v>44989.0</v>
       </c>
-      <c r="C111" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D111" s="21" t="s">
+      <c r="C111" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D111" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="E111" s="21" t="s">
+      <c r="E111" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="F111" s="21">
+      <c r="F111" s="22">
         <v>7050.0</v>
       </c>
       <c r="G111" s="13" t="s">
@@ -3838,22 +3805,22 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="18" t="s">
+      <c r="A113" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B113" s="19">
+      <c r="B113" s="20">
         <v>44996.0</v>
       </c>
-      <c r="C113" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D113" s="21" t="s">
+      <c r="C113" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D113" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E113" s="21" t="s">
+      <c r="E113" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F113" s="21">
+      <c r="F113" s="22">
         <v>6957.0</v>
       </c>
       <c r="G113" s="13" t="s">
@@ -3884,22 +3851,22 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="18" t="s">
+      <c r="A115" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B115" s="19">
+      <c r="B115" s="20">
         <v>45003.0</v>
       </c>
-      <c r="C115" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D115" s="21" t="s">
+      <c r="C115" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D115" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E115" s="21" t="s">
+      <c r="E115" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F115" s="21">
+      <c r="F115" s="22">
         <v>5985.0</v>
       </c>
       <c r="G115" s="13" t="s">
@@ -3930,22 +3897,22 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="18" t="s">
+      <c r="A117" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B117" s="19">
+      <c r="B117" s="20">
         <v>45010.0</v>
       </c>
-      <c r="C117" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D117" s="21" t="s">
+      <c r="C117" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D117" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E117" s="21" t="s">
+      <c r="E117" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F117" s="21">
+      <c r="F117" s="22">
         <v>5942.0</v>
       </c>
       <c r="G117" s="13" t="s">
@@ -3976,22 +3943,22 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="18" t="s">
+      <c r="A119" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B119" s="19">
+      <c r="B119" s="20">
         <v>45024.0</v>
       </c>
-      <c r="C119" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D119" s="21" t="s">
+      <c r="C119" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D119" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E119" s="21" t="s">
+      <c r="E119" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F119" s="21">
+      <c r="F119" s="22">
         <v>5432.0</v>
       </c>
       <c r="G119" s="13" t="s">
@@ -4022,22 +3989,22 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="18" t="s">
+      <c r="A121" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B121" s="19">
+      <c r="B121" s="20">
         <v>45031.0</v>
       </c>
-      <c r="C121" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D121" s="21" t="s">
+      <c r="C121" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D121" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E121" s="21" t="s">
+      <c r="E121" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F121" s="21">
+      <c r="F121" s="22">
         <v>6338.0</v>
       </c>
       <c r="G121" s="13" t="s">
@@ -4068,22 +4035,22 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="18" t="s">
+      <c r="A123" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B123" s="19">
+      <c r="B123" s="20">
         <v>45038.0</v>
       </c>
-      <c r="C123" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D123" s="21" t="s">
+      <c r="C123" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D123" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E123" s="21" t="s">
+      <c r="E123" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F123" s="21">
+      <c r="F123" s="22">
         <v>5556.0</v>
       </c>
       <c r="G123" s="13" t="s">
@@ -4114,22 +4081,22 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="18" t="s">
+      <c r="A125" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B125" s="19">
+      <c r="B125" s="20">
         <v>45045.0</v>
       </c>
-      <c r="C125" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D125" s="21" t="s">
+      <c r="C125" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D125" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E125" s="21" t="s">
+      <c r="E125" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F125" s="21">
+      <c r="F125" s="22">
         <v>6481.0</v>
       </c>
       <c r="G125" s="13" t="s">
@@ -4160,22 +4127,22 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="18" t="s">
+      <c r="A127" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B127" s="19">
+      <c r="B127" s="20">
         <v>45052.0</v>
       </c>
-      <c r="C127" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D127" s="21" t="s">
+      <c r="C127" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D127" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E127" s="21" t="s">
+      <c r="E127" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F127" s="21">
+      <c r="F127" s="22">
         <v>6195.0</v>
       </c>
       <c r="G127" s="13" t="s">
@@ -4206,22 +4173,22 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="18" t="s">
+      <c r="A129" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B129" s="19">
+      <c r="B129" s="20">
         <v>45059.0</v>
       </c>
-      <c r="C129" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D129" s="21" t="s">
+      <c r="C129" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D129" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E129" s="21" t="s">
+      <c r="E129" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F129" s="21">
+      <c r="F129" s="22">
         <v>6303.0</v>
       </c>
       <c r="G129" s="13" t="s">
@@ -4252,22 +4219,22 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="18" t="s">
+      <c r="A131" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B131" s="19">
+      <c r="B131" s="20">
         <v>45066.0</v>
       </c>
-      <c r="C131" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="D131" s="21" t="s">
+      <c r="C131" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D131" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E131" s="21" t="s">
+      <c r="E131" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="F131" s="21">
+      <c r="F131" s="22">
         <v>5887.0</v>
       </c>
       <c r="G131" s="13" t="s">
@@ -4298,22 +4265,22 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="18" t="s">
+      <c r="A133" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B133" s="19">
+      <c r="B133" s="20">
         <v>45073.0</v>
       </c>
-      <c r="C133" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="D133" s="21" t="s">
+      <c r="C133" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D133" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E133" s="21" t="s">
+      <c r="E133" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F133" s="21">
+      <c r="F133" s="22">
         <v>6128.0</v>
       </c>
       <c r="G133" s="13" t="s">
@@ -4367,22 +4334,22 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="22" t="s">
+      <c r="A136" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B136" s="23">
+      <c r="B136" s="24">
         <v>44952.0</v>
       </c>
-      <c r="C136" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="D136" s="25" t="s">
+      <c r="C136" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="D136" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E136" s="25" t="s">
+      <c r="E136" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F136" s="25">
+      <c r="F136" s="26">
         <v>0.0</v>
       </c>
       <c r="G136" s="8" t="s">
@@ -4390,22 +4357,22 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="18" t="s">
+      <c r="A137" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B137" s="19">
+      <c r="B137" s="20">
         <v>44959.0</v>
       </c>
-      <c r="C137" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D137" s="21" t="s">
+      <c r="C137" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D137" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E137" s="21" t="s">
+      <c r="E137" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F137" s="21">
+      <c r="F137" s="22">
         <v>5600.0</v>
       </c>
       <c r="G137" s="13" t="s">
@@ -4436,22 +4403,22 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="18" t="s">
+      <c r="A139" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B139" s="19">
+      <c r="B139" s="20">
         <v>44973.0</v>
       </c>
-      <c r="C139" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D139" s="21" t="s">
+      <c r="C139" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D139" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E139" s="21" t="s">
+      <c r="E139" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F139" s="21">
+      <c r="F139" s="22">
         <v>9491.0</v>
       </c>
       <c r="G139" s="13" t="s">
@@ -4482,22 +4449,22 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="18" t="s">
+      <c r="A141" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B141" s="19">
+      <c r="B141" s="20">
         <v>44987.0</v>
       </c>
-      <c r="C141" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D141" s="21" t="s">
+      <c r="C141" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D141" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E141" s="21" t="s">
+      <c r="E141" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="F141" s="21">
+      <c r="F141" s="22">
         <v>6365.0</v>
       </c>
       <c r="G141" s="13" t="s">
@@ -4528,22 +4495,22 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="18" t="s">
+      <c r="A143" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B143" s="19">
+      <c r="B143" s="20">
         <v>45001.0</v>
       </c>
-      <c r="C143" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D143" s="21" t="s">
+      <c r="C143" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D143" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E143" s="21" t="s">
+      <c r="E143" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F143" s="21">
+      <c r="F143" s="22">
         <v>5851.0</v>
       </c>
       <c r="G143" s="13" t="s">
@@ -4574,22 +4541,22 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="18" t="s">
+      <c r="A145" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B145" s="19">
+      <c r="B145" s="20">
         <v>45015.0</v>
       </c>
-      <c r="C145" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D145" s="21" t="s">
+      <c r="C145" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D145" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E145" s="21" t="s">
+      <c r="E145" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F145" s="21">
+      <c r="F145" s="22">
         <v>6117.0</v>
       </c>
       <c r="G145" s="13" t="s">
@@ -4597,22 +4564,22 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="22" t="s">
+      <c r="A146" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B146" s="23">
+      <c r="B146" s="24">
         <v>45022.0</v>
       </c>
-      <c r="C146" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="D146" s="25" t="s">
+      <c r="C146" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="D146" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E146" s="25" t="s">
+      <c r="E146" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F146" s="25">
+      <c r="F146" s="26">
         <v>0.0</v>
       </c>
       <c r="G146" s="8" t="s">
@@ -4620,22 +4587,22 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="18" t="s">
+      <c r="A147" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B147" s="19">
+      <c r="B147" s="20">
         <v>45029.0</v>
       </c>
-      <c r="C147" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D147" s="21" t="s">
+      <c r="C147" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D147" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="E147" s="21" t="s">
+      <c r="E147" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F147" s="21">
+      <c r="F147" s="22">
         <v>7018.0</v>
       </c>
       <c r="G147" s="13" t="s">
@@ -4666,22 +4633,22 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="18" t="s">
+      <c r="A149" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B149" s="19">
+      <c r="B149" s="20">
         <v>45043.0</v>
       </c>
-      <c r="C149" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D149" s="21" t="s">
+      <c r="C149" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D149" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E149" s="21" t="s">
+      <c r="E149" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F149" s="21">
+      <c r="F149" s="22">
         <v>7074.0</v>
       </c>
       <c r="G149" s="13" t="s">
@@ -4712,22 +4679,22 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="18" t="s">
+      <c r="A151" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B151" s="19">
+      <c r="B151" s="20">
         <v>45057.0</v>
       </c>
-      <c r="C151" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D151" s="21" t="s">
+      <c r="C151" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D151" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E151" s="21" t="s">
+      <c r="E151" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F151" s="21">
+      <c r="F151" s="22">
         <v>6793.0</v>
       </c>
       <c r="G151" s="13" t="s">
@@ -4758,22 +4725,22 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="22" t="s">
+      <c r="A153" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B153" s="23">
+      <c r="B153" s="24">
         <v>45092.0</v>
       </c>
-      <c r="C153" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="D153" s="25" t="s">
+      <c r="C153" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="D153" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E153" s="25" t="s">
+      <c r="E153" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="F153" s="25">
+      <c r="F153" s="26">
         <v>0.0</v>
       </c>
       <c r="G153" s="13" t="s">
@@ -4781,22 +4748,22 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="22" t="s">
+      <c r="A154" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B154" s="23">
+      <c r="B154" s="24">
         <v>45197.0</v>
       </c>
-      <c r="C154" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="D154" s="25" t="s">
+      <c r="C154" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="D154" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="E154" s="25" t="s">
+      <c r="E154" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="F154" s="25">
+      <c r="F154" s="26">
         <v>0.0</v>
       </c>
       <c r="G154" s="8" t="s">
@@ -4804,22 +4771,22 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="22" t="s">
+      <c r="A155" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B155" s="23">
+      <c r="B155" s="24">
         <v>45204.0</v>
       </c>
-      <c r="C155" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="D155" s="25" t="s">
+      <c r="C155" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="D155" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E155" s="25" t="s">
+      <c r="E155" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="F155" s="25">
+      <c r="F155" s="26">
         <v>0.0</v>
       </c>
       <c r="G155" s="13" t="s">
@@ -4827,22 +4794,22 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="22" t="s">
+      <c r="A156" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B156" s="23">
+      <c r="B156" s="24">
         <v>45225.0</v>
       </c>
-      <c r="C156" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="D156" s="25" t="s">
+      <c r="C156" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="D156" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="E156" s="25" t="s">
+      <c r="E156" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="F156" s="25">
+      <c r="F156" s="26">
         <v>0.0</v>
       </c>
       <c r="G156" s="8" t="s">
@@ -4850,22 +4817,22 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="22" t="s">
+      <c r="A157" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B157" s="23">
+      <c r="B157" s="24">
         <v>45337.0</v>
       </c>
-      <c r="C157" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="D157" s="25" t="s">
+      <c r="C157" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="D157" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E157" s="25" t="s">
+      <c r="E157" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="F157" s="25">
+      <c r="F157" s="26">
         <v>0.0</v>
       </c>
       <c r="G157" s="13" t="s">
@@ -4873,22 +4840,22 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="22" t="s">
+      <c r="A158" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B158" s="23">
+      <c r="B158" s="24">
         <v>45421.0</v>
       </c>
-      <c r="C158" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="D158" s="25" t="s">
+      <c r="C158" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="D158" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="E158" s="25" t="s">
+      <c r="E158" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="F158" s="25">
+      <c r="F158" s="26">
         <v>0.0</v>
       </c>
       <c r="G158" s="8" t="s">
@@ -4896,22 +4863,22 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="22" t="s">
+      <c r="A159" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B159" s="23">
+      <c r="B159" s="24">
         <v>45687.0</v>
       </c>
-      <c r="C159" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="D159" s="25" t="s">
+      <c r="C159" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="D159" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="E159" s="25" t="s">
+      <c r="E159" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="F159" s="25">
+      <c r="F159" s="26">
         <v>0.0</v>
       </c>
       <c r="G159" s="13" t="s">
@@ -4942,22 +4909,22 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="18" t="s">
+      <c r="A161" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B161" s="19">
+      <c r="B161" s="20">
         <v>44978.0</v>
       </c>
-      <c r="C161" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="D161" s="26" t="s">
+      <c r="C161" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D161" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="E161" s="21" t="s">
+      <c r="E161" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="F161" s="21">
+      <c r="F161" s="22">
         <v>2941.0</v>
       </c>
       <c r="G161" s="13" t="s">
@@ -4988,22 +4955,22 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="18" t="s">
+      <c r="A163" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B163" s="19">
+      <c r="B163" s="20">
         <v>44985.0</v>
       </c>
-      <c r="C163" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="D163" s="26" t="s">
+      <c r="C163" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D163" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="E163" s="21" t="s">
+      <c r="E163" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="F163" s="21">
+      <c r="F163" s="22">
         <v>2822.0</v>
       </c>
       <c r="G163" s="13" t="s">
@@ -5034,22 +5001,22 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="18" t="s">
+      <c r="A165" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B165" s="19">
+      <c r="B165" s="20">
         <v>44999.0</v>
       </c>
-      <c r="C165" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="D165" s="21" t="s">
+      <c r="C165" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D165" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="E165" s="21" t="s">
+      <c r="E165" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="F165" s="21">
+      <c r="F165" s="22">
         <v>4382.0</v>
       </c>
       <c r="G165" s="13" t="s">
@@ -5080,22 +5047,22 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="18" t="s">
+      <c r="A167" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B167" s="19">
+      <c r="B167" s="20">
         <v>45013.0</v>
       </c>
-      <c r="C167" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="D167" s="21" t="s">
+      <c r="C167" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D167" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="E167" s="21" t="s">
+      <c r="E167" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="F167" s="21">
+      <c r="F167" s="22">
         <v>2536.0</v>
       </c>
       <c r="G167" s="13" t="s">
@@ -5126,22 +5093,22 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="18" t="s">
+      <c r="A169" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B169" s="19">
+      <c r="B169" s="20">
         <v>45020.0</v>
       </c>
-      <c r="C169" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="D169" s="21" t="s">
+      <c r="C169" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D169" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="E169" s="21" t="s">
+      <c r="E169" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="F169" s="21">
+      <c r="F169" s="22">
         <v>2879.0</v>
       </c>
       <c r="G169" s="13" t="s">
@@ -5172,22 +5139,22 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="18" t="s">
+      <c r="A171" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B171" s="19">
+      <c r="B171" s="20">
         <v>45034.0</v>
       </c>
-      <c r="C171" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="D171" s="21" t="s">
+      <c r="C171" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D171" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="E171" s="21" t="s">
+      <c r="E171" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="F171" s="21">
+      <c r="F171" s="22">
         <v>3760.0</v>
       </c>
       <c r="G171" s="13" t="s">
@@ -5218,22 +5185,22 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="18" t="s">
+      <c r="A173" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B173" s="19">
+      <c r="B173" s="20">
         <v>45041.0</v>
       </c>
-      <c r="C173" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="D173" s="21" t="s">
+      <c r="C173" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D173" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="E173" s="21" t="s">
+      <c r="E173" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="F173" s="21">
+      <c r="F173" s="22">
         <v>5860.0</v>
       </c>
       <c r="G173" s="13" t="s">
@@ -5264,22 +5231,22 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" s="18" t="s">
+      <c r="A175" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B175" s="19">
+      <c r="B175" s="20">
         <v>45055.0</v>
       </c>
-      <c r="C175" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="D175" s="21" t="s">
+      <c r="C175" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D175" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="E175" s="21" t="s">
+      <c r="E175" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="F175" s="21">
+      <c r="F175" s="22">
         <v>1632.0</v>
       </c>
       <c r="G175" s="13" t="s">
@@ -5310,22 +5277,22 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="18" t="s">
+      <c r="A177" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B177" s="19">
+      <c r="B177" s="20">
         <v>45062.0</v>
       </c>
-      <c r="C177" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="D177" s="21" t="s">
+      <c r="C177" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D177" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="E177" s="21" t="s">
+      <c r="E177" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="F177" s="21">
+      <c r="F177" s="22">
         <v>1488.0</v>
       </c>
       <c r="G177" s="13" t="s">
@@ -5356,25 +5323,25 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" s="27" t="s">
+      <c r="A179" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B179" s="28">
+      <c r="B179" s="29">
         <v>45069.0</v>
       </c>
-      <c r="C179" s="29">
-        <v>3.0</v>
-      </c>
-      <c r="D179" s="30" t="s">
+      <c r="C179" s="30">
+        <v>3.0</v>
+      </c>
+      <c r="D179" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="E179" s="30" t="s">
+      <c r="E179" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="F179" s="30">
+      <c r="F179" s="31">
         <v>2353.0</v>
       </c>
-      <c r="G179" s="31" t="s">
+      <c r="G179" s="32" t="s">
         <v>10</v>
       </c>
     </row>
@@ -5439,7 +5406,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="5">
@@ -5462,7 +5429,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="10">
@@ -5485,7 +5452,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="33" t="s">
         <v>105</v>
       </c>
       <c r="B4" s="5">
@@ -5508,7 +5475,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="34" t="s">
         <v>105</v>
       </c>
       <c r="B5" s="10">
@@ -5531,7 +5498,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="33" t="s">
         <v>105</v>
       </c>
       <c r="B6" s="5">
@@ -5554,7 +5521,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="34" t="s">
         <v>60</v>
       </c>
       <c r="B7" s="10">
@@ -5577,7 +5544,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="33" t="s">
         <v>60</v>
       </c>
       <c r="B8" s="5">
@@ -5600,7 +5567,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="34" t="s">
         <v>85</v>
       </c>
       <c r="B9" s="10">
@@ -5623,7 +5590,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="33" t="s">
         <v>85</v>
       </c>
       <c r="B10" s="5">
@@ -5646,7 +5613,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="34" t="s">
         <v>85</v>
       </c>
       <c r="B11" s="10">
@@ -5669,7 +5636,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="33" t="s">
         <v>85</v>
       </c>
       <c r="B12" s="5">
@@ -5692,7 +5659,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="34" t="s">
         <v>85</v>
       </c>
       <c r="B13" s="10">
@@ -5715,7 +5682,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="33" t="s">
         <v>85</v>
       </c>
       <c r="B14" s="5">
@@ -5738,7 +5705,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="34" t="s">
         <v>91</v>
       </c>
       <c r="B15" s="10">
@@ -5761,7 +5728,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="33" t="s">
         <v>91</v>
       </c>
       <c r="B16" s="5">
@@ -5784,7 +5751,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="34" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="10">
@@ -5807,7 +5774,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="33" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="5">
@@ -5830,7 +5797,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="34" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="10">
@@ -5853,7 +5820,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="33" t="s">
         <v>105</v>
       </c>
       <c r="B20" s="5">
@@ -5876,7 +5843,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="34" t="s">
         <v>60</v>
       </c>
       <c r="B21" s="10">
@@ -5899,7 +5866,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="33" t="s">
         <v>60</v>
       </c>
       <c r="B22" s="5">
@@ -5922,7 +5889,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="34" t="s">
         <v>105</v>
       </c>
       <c r="B23" s="10">
@@ -5945,7 +5912,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="33" t="s">
         <v>105</v>
       </c>
       <c r="B24" s="5">
@@ -5968,7 +5935,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="34" t="s">
         <v>60</v>
       </c>
       <c r="B25" s="10">
@@ -5991,37 +5958,106 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="35">
+      <c r="B26" s="5">
         <v>45504.0</v>
       </c>
-      <c r="C26" s="36">
+      <c r="C26" s="6">
         <v>4.0</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="E26" s="37" t="s">
+      <c r="E26" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="F26" s="36">
+      <c r="F26" s="6">
         <v>1062.0</v>
       </c>
-      <c r="G26" s="38" t="s">
+      <c r="G26" s="8" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="20">
+        <v>45794.0</v>
+      </c>
+      <c r="C27" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" s="21">
+        <v>5696.0</v>
+      </c>
+      <c r="G27" s="36" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="15">
+        <v>45787.0</v>
+      </c>
+      <c r="C28" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="F28" s="16">
+        <v>5541.0</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="29">
+        <v>45097.0</v>
+      </c>
+      <c r="C29" s="30">
+        <v>3.0</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="F29" s="30">
+        <v>2377.0</v>
+      </c>
+      <c r="G29" s="39" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="A2:A26">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="A2:A29">
       <formula1>"Show Champion,Show,Show! Music Core,M Countdown,Inkigayo,Music Bank"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B26">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B29">
       <formula1>OR(NOT(ISERROR(DATEVALUE(B2))), AND(ISNUMBER(B2), LEFT(CELL("format", B2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C2:C26 F2:F26">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C2:C29 F2:F29">
       <formula1>AND(ISNUMBER(C2),(NOT(OR(NOT(ISERROR(DATEVALUE(C2))), AND(ISNUMBER(C2), LEFT(CELL("format", C2))="D")))))</formula1>
     </dataValidation>
   </dataValidations>
@@ -6135,22 +6171,22 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="20">
         <v>45083.0</v>
       </c>
-      <c r="C5" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="22">
         <v>6606.0</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -6181,22 +6217,22 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="20">
         <v>45105.0</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="21">
         <v>1.0</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="22">
         <v>5310.0</v>
       </c>
       <c r="G7" s="13" t="s">
@@ -6214,7 +6250,7 @@
         <v>3.0</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>146</v>
@@ -6227,22 +6263,22 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="20">
         <v>45717.0</v>
       </c>
-      <c r="C9" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="F9" s="21">
+      <c r="E9" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="F9" s="22">
         <v>5836.0</v>
       </c>
       <c r="G9" s="13" t="s">
@@ -6263,7 +6299,7 @@
         <v>148</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F10" s="17">
         <v>4154.0</v>
@@ -6273,22 +6309,22 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="20">
         <v>45703.0</v>
       </c>
-      <c r="C11" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="D11" s="21" t="s">
+      <c r="C11" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D11" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="F11" s="21">
+      <c r="E11" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="F11" s="22">
         <v>3972.0</v>
       </c>
       <c r="G11" s="13" t="s">
@@ -6309,7 +6345,7 @@
         <v>148</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F12" s="17">
         <v>5340.0</v>
@@ -6319,22 +6355,22 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="20">
         <v>45682.0</v>
       </c>
-      <c r="C13" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D13" s="21" t="s">
+      <c r="C13" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="F13" s="21">
+      <c r="E13" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" s="22">
         <v>5815.0</v>
       </c>
       <c r="G13" s="13" t="s">
@@ -6355,7 +6391,7 @@
         <v>148</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F14" s="17">
         <v>5777.0</v>
@@ -6365,22 +6401,22 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="20">
         <v>45680.0</v>
       </c>
-      <c r="C15" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D15" s="21" t="s">
+      <c r="C15" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D15" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="F15" s="21">
+      <c r="E15" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="F15" s="22">
         <v>6077.0</v>
       </c>
       <c r="G15" s="13" t="s">
@@ -6401,7 +6437,7 @@
         <v>148</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F16" s="17">
         <v>9500.0</v>
@@ -6411,22 +6447,22 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="20">
         <v>45802.0</v>
       </c>
-      <c r="C17" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D17" s="21" t="s">
+      <c r="C17" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D17" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="E17" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="F17" s="21">
+      <c r="E17" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="F17" s="22">
         <v>3857.0</v>
       </c>
       <c r="G17" s="13" t="s">
@@ -6447,7 +6483,7 @@
         <v>148</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F18" s="17">
         <v>5869.0</v>
@@ -6457,22 +6493,22 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="20">
         <v>45674.0</v>
       </c>
-      <c r="C19" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="D19" s="21" t="s">
+      <c r="C19" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D19" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="E19" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="F19" s="21">
+      <c r="E19" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="F19" s="22">
         <v>3922.0</v>
       </c>
       <c r="G19" s="13" t="s">
@@ -6490,7 +6526,7 @@
         <v>1.0</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>155</v>
@@ -6595,57 +6631,126 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="20">
         <v>45518.0</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="21">
         <v>5.0</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F25" s="22">
+        <v>1095.0</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="15">
+        <v>45504.0</v>
+      </c>
+      <c r="C26" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="F26" s="17">
+        <v>1062.0</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="20">
+        <v>45794.0</v>
+      </c>
+      <c r="C27" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" s="22">
+        <v>5696.0</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="15">
+        <v>45787.0</v>
+      </c>
+      <c r="C28" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="F28" s="17">
+        <v>5541.0</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="29">
+        <v>45097.0</v>
+      </c>
+      <c r="C29" s="30">
+        <v>3.0</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="E29" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="E25" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="F25" s="21">
-        <v>1095.0</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="40">
-        <v>45504.0</v>
-      </c>
-      <c r="C26" s="41">
-        <v>4.0</v>
-      </c>
-      <c r="D26" s="42" t="s">
-        <v>167</v>
-      </c>
-      <c r="E26" s="42" t="s">
-        <v>163</v>
-      </c>
-      <c r="F26" s="42">
-        <v>1062.0</v>
-      </c>
-      <c r="G26" s="38" t="s">
+      <c r="F29" s="31">
+        <v>2377.0</v>
+      </c>
+      <c r="G29" s="32" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B26">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B29">
       <formula1>OR(NOT(ISERROR(DATEVALUE(B2))), AND(ISNUMBER(B2), LEFT(CELL("format", B2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C2:C26">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C2:C29">
       <formula1>AND(ISNUMBER(C2),(NOT(OR(NOT(ISERROR(DATEVALUE(C2))), AND(ISNUMBER(C2), LEFT(CELL("format", C2))="D")))))</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Downloaded & Feature Extraction finished
</commit_message>
<xml_diff>
--- a/data/manual_changes/manual_awards.xlsx
+++ b/data/manual_changes/manual_awards.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="179">
   <si>
     <t>show</t>
   </si>
@@ -519,6 +519,15 @@
     <t>Wild Heart</t>
   </si>
   <si>
+    <t>Lee Jegyu</t>
+  </si>
+  <si>
+    <t>Mironi</t>
+  </si>
+  <si>
+    <t>2024_show</t>
+  </si>
+  <si>
     <t>Hwang Karam</t>
   </si>
   <si>
@@ -535,6 +544,12 @@
   </si>
   <si>
     <t>LUN8</t>
+  </si>
+  <si>
+    <t>Lee Jegyu, Lazybone</t>
+  </si>
+  <si>
+    <t>Miruni</t>
   </si>
 </sst>
 </file>
@@ -571,7 +586,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border/>
     <border>
       <left style="thin">
@@ -769,11 +784,53 @@
         <color rgb="FF284E3F"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -888,10 +945,22 @@
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -985,7 +1054,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G29" displayName="Table2" name="Table2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G30" displayName="Table2" name="Table2" id="2">
   <tableColumns count="7">
     <tableColumn name="show" id="1"/>
     <tableColumn name="date" id="2"/>
@@ -1000,7 +1069,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G29" displayName="Table3" name="Table3" id="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G30" displayName="Table3" name="Table3" id="3">
   <tableColumns count="7">
     <tableColumn name="show" id="1"/>
     <tableColumn name="date" id="2"/>
@@ -6027,37 +6096,60 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="B29" s="29">
+      <c r="B29" s="20">
         <v>45097.0</v>
       </c>
-      <c r="C29" s="30">
-        <v>3.0</v>
-      </c>
-      <c r="D29" s="31" t="s">
+      <c r="C29" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D29" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="F29" s="30">
+      <c r="F29" s="21">
         <v>2377.0</v>
       </c>
-      <c r="G29" s="39" t="s">
+      <c r="G29" s="36" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="39">
+        <v>45559.0</v>
+      </c>
+      <c r="C30" s="40">
+        <v>2.0</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="F30" s="40">
+        <v>4582.0</v>
+      </c>
+      <c r="G30" s="42" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="A2:A29">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="A2:A30">
       <formula1>"Show Champion,Show,Show! Music Core,M Countdown,Inkigayo,Music Bank"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B29">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B30">
       <formula1>OR(NOT(ISERROR(DATEVALUE(B2))), AND(ISNUMBER(B2), LEFT(CELL("format", B2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C2:C29 F2:F29">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C2:C30 F2:F30">
       <formula1>AND(ISNUMBER(C2),(NOT(OR(NOT(ISERROR(DATEVALUE(C2))), AND(ISNUMBER(C2), LEFT(CELL("format", C2))="D")))))</formula1>
     </dataValidation>
   </dataValidations>
@@ -6250,7 +6342,7 @@
         <v>3.0</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>146</v>
@@ -6276,7 +6368,7 @@
         <v>148</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F9" s="22">
         <v>5836.0</v>
@@ -6299,7 +6391,7 @@
         <v>148</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F10" s="17">
         <v>4154.0</v>
@@ -6322,7 +6414,7 @@
         <v>148</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F11" s="22">
         <v>3972.0</v>
@@ -6345,7 +6437,7 @@
         <v>148</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F12" s="17">
         <v>5340.0</v>
@@ -6368,7 +6460,7 @@
         <v>148</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F13" s="22">
         <v>5815.0</v>
@@ -6391,7 +6483,7 @@
         <v>148</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F14" s="17">
         <v>5777.0</v>
@@ -6414,7 +6506,7 @@
         <v>148</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F15" s="22">
         <v>6077.0</v>
@@ -6437,7 +6529,7 @@
         <v>148</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F16" s="17">
         <v>9500.0</v>
@@ -6460,7 +6552,7 @@
         <v>148</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F17" s="22">
         <v>3857.0</v>
@@ -6483,7 +6575,7 @@
         <v>148</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F18" s="17">
         <v>5869.0</v>
@@ -6506,7 +6598,7 @@
         <v>148</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F19" s="22">
         <v>3922.0</v>
@@ -6526,7 +6618,7 @@
         <v>1.0</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>155</v>
@@ -6641,7 +6733,7 @@
         <v>5.0</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E25" s="22" t="s">
         <v>163</v>
@@ -6664,7 +6756,7 @@
         <v>4.0</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E26" s="17" t="s">
         <v>163</v>
@@ -6687,7 +6779,7 @@
         <v>2.0</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E27" s="22" t="s">
         <v>165</v>
@@ -6710,7 +6802,7 @@
         <v>2.0</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>165</v>
@@ -6723,34 +6815,57 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B29" s="29">
+      <c r="B29" s="20">
         <v>45097.0</v>
       </c>
-      <c r="C29" s="30">
-        <v>3.0</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>173</v>
-      </c>
-      <c r="E29" s="31" t="s">
+      <c r="C29" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="E29" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="F29" s="31">
+      <c r="F29" s="22">
         <v>2377.0</v>
       </c>
-      <c r="G29" s="32" t="s">
+      <c r="G29" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="39">
+        <v>45559.0</v>
+      </c>
+      <c r="C30" s="40">
+        <v>2.0</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>178</v>
+      </c>
+      <c r="F30" s="41">
+        <v>4582.0</v>
+      </c>
+      <c r="G30" s="42" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B29">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B2:B30">
       <formula1>OR(NOT(ISERROR(DATEVALUE(B2))), AND(ISNUMBER(B2), LEFT(CELL("format", B2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C2:C29">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C2:C30">
       <formula1>AND(ISNUMBER(C2),(NOT(OR(NOT(ISERROR(DATEVALUE(C2))), AND(ISNUMBER(C2), LEFT(CELL("format", C2))="D")))))</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>